<commit_message>
Added Form with mock data
</commit_message>
<xml_diff>
--- a/Campaign Form.xlsx
+++ b/Campaign Form.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Address</t>
   </si>
@@ -96,6 +96,42 @@
   </si>
   <si>
     <t>Incurred</t>
+  </si>
+  <si>
+    <t>PT-PAC of MO</t>
+  </si>
+  <si>
+    <t>205 E Capitol</t>
+  </si>
+  <si>
+    <t>Jefferson City</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>A Better Missouri</t>
+  </si>
+  <si>
+    <t>48 Willmore Rd</t>
+  </si>
+  <si>
+    <t>St Louis</t>
+  </si>
+  <si>
+    <t>City of St Louis</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Bushmeyer</t>
+  </si>
+  <si>
+    <t>Ed</t>
   </si>
 </sst>
 </file>
@@ -139,9 +175,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,57 +459,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>65101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43697</v>
+      </c>
+      <c r="K2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>65101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2">
+        <v>43666</v>
+      </c>
+      <c r="K3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>65101</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43697</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>63109</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2">
+        <v>43637</v>
+      </c>
+      <c r="K5">
+        <v>200</v>
+      </c>
+      <c r="L5">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -485,13 +652,13 @@
           <x14:formula1>
             <xm:f>'Drop Down Lists (Don''t Touch)'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Drop Down Lists (Don''t Touch)'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>